<commit_message>
First Commit - Automation Framework(Amazon)
</commit_message>
<xml_diff>
--- a/resources/test-data/AmazonSearchTestData.xlsx
+++ b/resources/test-data/AmazonSearchTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="14835" windowHeight="3405"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14835" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Clothing" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="clothing1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="E1:I11"/>
 </workbook>
 </file>
 
@@ -553,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>